<commit_message>
fix excel with HDF5 sizes
</commit_message>
<xml_diff>
--- a/assignment5/comparative_table.xlsx
+++ b/assignment5/comparative_table.xlsx
@@ -5,18 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarv\AppData\Roaming\MobaXterm\slash\RemoteFiles\140982_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UTSA\Spring_2024\High Performance Computing\Week_6\HW5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87D0399-5021-4682-B491-A3905FAA5037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2118A193-5234-404D-A427-0140463CB21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="qZ78jfYSNy+LbUd5ShYddO09p3klKXBL4YMz67vRVtw="/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Matrix</t>
   </si>
@@ -68,13 +79,19 @@
   <si>
     <t>E</t>
   </si>
+  <si>
+    <t>HDF5 Size</t>
+  </si>
+  <si>
+    <t>Total HDF5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -108,12 +125,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -156,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,7 +199,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -394,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -407,14 +442,14 @@
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" customWidth="1"/>
-    <col min="10" max="26" width="8.6640625" customWidth="1"/>
+    <col min="6" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
+    <col min="10" max="10" width="24.109375" customWidth="1"/>
+    <col min="11" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,104 +468,116 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="7">
         <v>3.07254958152771</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="11">
         <v>0.14608359336853</v>
       </c>
       <c r="D2" s="7">
         <v>1.39924836158752</v>
       </c>
       <c r="E2" s="3">
-        <v>48</v>
+        <v>47.68</v>
       </c>
       <c r="F2" s="4">
-        <v>191</v>
-      </c>
-      <c r="G2" s="3">
+        <v>190.73</v>
+      </c>
+      <c r="G2" s="8">
+        <v>18.942799999999998</v>
+      </c>
+      <c r="H2" s="3">
         <v>0.61458999999999997</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="10">
         <v>6.4530000000000004E-2</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>0.34023999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="7">
         <v>3.1581995487213099</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="11">
         <v>1.5682220458984299E-2</v>
       </c>
       <c r="D3" s="7">
         <v>0.73623394966125399</v>
       </c>
       <c r="E3" s="3">
-        <v>96</v>
+        <v>95.37</v>
       </c>
       <c r="F3" s="4">
-        <v>24</v>
-      </c>
-      <c r="G3" s="3">
+        <v>23.84</v>
+      </c>
+      <c r="G3" s="9">
+        <v>16.109100000000002</v>
+      </c>
+      <c r="H3" s="3">
         <v>0.76910999999999996</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="10">
         <v>9.5860000000000008E-3</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="6">
         <v>0.12861</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7">
         <v>11.7983934879302</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="11">
         <v>0.13498711585998499</v>
       </c>
       <c r="D4" s="7">
         <v>0.71239733695983798</v>
       </c>
       <c r="E4" s="3">
-        <v>597</v>
+        <v>596.04999999999995</v>
       </c>
       <c r="F4" s="4">
-        <v>191</v>
-      </c>
-      <c r="G4" s="3">
+        <v>190.73</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.3967</v>
+      </c>
+      <c r="H4" s="3">
         <v>6.3051000000000004</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="10">
         <v>6.31216E-2</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>0.21088999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -540,7 +587,7 @@
       <c r="C5" s="7">
         <v>1.2826919555664E-3</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="11">
         <v>1.9018650054931599E-3</v>
       </c>
       <c r="E5" s="3">
@@ -549,17 +596,20 @@
       <c r="F5" s="4">
         <v>3.28E-4</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="8">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="H5" s="3">
         <v>8.6899999999999998E-4</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>5.6599999999999999E-4</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="10">
         <v>3.9399999999999998E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -569,7 +619,7 @@
       <c r="C6" s="7">
         <v>9.9778175354003906E-4</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="11">
         <v>2.4747848510742101E-4</v>
       </c>
       <c r="E6" s="3">
@@ -578,26 +628,41 @@
       <c r="F6" s="4">
         <v>1.44E-4</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="8">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="H6" s="3">
         <v>4.0749999999999998E-4</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>3.5570000000000003E-4</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="10">
         <v>7.3433E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f>SUM(G2:G6)</f>
+        <v>35.448766000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>33.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>